<commit_message>
N64RGBv1/v2 misc updates  (thanks to iFixRetro for giving feedback here!!!): - bugfix BOM and silkscreen (N64RGBv2) - silkscreen update to distinguish between MaxII and MaxV setup avoiding assembly mistakes - move power regulator to BOT copper side (N64RGBv1) - additional jumper J1 to select between 240LE and 570LE CPLD (for proper usage of the 5M240ZT)
</commit_message>
<xml_diff>
--- a/generalRGBmod/Main-PCB/v1/BOM_n64rgbv1.xlsx
+++ b/generalRGBmod/Main-PCB/v1/BOM_n64rgbv1.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ToshibaHDWM110/borti4938/Documents/Workspaces/Git/N64RGB/generalRGBmod/Main-PCB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Peter\Documents\Workspaces\Git\N64RGB\generalRGBmod\Main-PCB\v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14445" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MaxV Setup" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="117">
   <si>
     <t>Designator</t>
   </si>
@@ -129,15 +129,6 @@
     <t>1.8V LDO regulator</t>
   </si>
   <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>(Jumper)</t>
-  </si>
-  <si>
-    <t>Leave J1 open</t>
-  </si>
-  <si>
     <t>ICs and Regulators</t>
   </si>
   <si>
@@ -225,12 +216,6 @@
     <t xml:space="preserve">Optional components for plug decoupling </t>
   </si>
   <si>
-    <t>C31</t>
-  </si>
-  <si>
-    <t>C32,C33</t>
-  </si>
-  <si>
     <t>10uF / 6.3V (10%)</t>
   </si>
   <si>
@@ -240,9 +225,6 @@
     <t>C0603C105K9R</t>
   </si>
   <si>
-    <t>GRM426X106K6.3L</t>
-  </si>
-  <si>
     <t>Remaining passive components</t>
   </si>
   <si>
@@ -348,31 +330,61 @@
     <t>4x 39ohm (1%)</t>
   </si>
   <si>
-    <t>Short J1</t>
-  </si>
-  <si>
     <t>EPM570T100C5N</t>
   </si>
   <si>
     <t>EPM240T100C5N</t>
   </si>
   <si>
-    <t>Alternative to EPM570T100 with less LEs</t>
-  </si>
-  <si>
-    <t>Alternative to 5M570ZT100 with less LEs</t>
-  </si>
-  <si>
     <t>280ohm (1%)</t>
   </si>
   <si>
     <t>RC0603FR-07280RL</t>
+  </si>
+  <si>
+    <t>Unpopulated Footprints</t>
+  </si>
+  <si>
+    <t>FB2</t>
+  </si>
+  <si>
+    <t>SMD1206/SMD0805</t>
+  </si>
+  <si>
+    <t>Alternative to 5M570ZT100 with less Les, leave J1 open</t>
+  </si>
+  <si>
+    <t>Close J1</t>
+  </si>
+  <si>
+    <t>C31,C32</t>
+  </si>
+  <si>
+    <t>C2,C3</t>
+  </si>
+  <si>
+    <t>SMD0805</t>
+  </si>
+  <si>
+    <t>GRM21BR60J106ME19L</t>
+  </si>
+  <si>
+    <t>Don't use FB2 in MaxV setup!!! Otherwise you'll harm your CPLD at first power cycle</t>
+  </si>
+  <si>
+    <t>U3,C31,C32</t>
+  </si>
+  <si>
+    <t>These components are for MaxV setup only!!! Leave them free.</t>
+  </si>
+  <si>
+    <t>Alternative to EPM570T100 with less Les, leave J1 open</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -917,17 +929,17 @@
     <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Besuchter Link" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
+    <cellStyle name="Link" xfId="42" builtinId="8"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1213,20 +1225,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="23.5" customWidth="1"/>
-    <col min="5" max="5" width="18.5" customWidth="1"/>
-    <col min="7" max="7" width="59.83203125" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="59.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1249,13 +1263,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1271,10 +1285,13 @@
       <c r="F4" t="s">
         <v>19</v>
       </c>
+      <c r="G4" t="s">
+        <v>108</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>18</v>
       </c>
@@ -1285,12 +1302,12 @@
         <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>24</v>
       </c>
@@ -1311,7 +1328,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7" t="s">
         <v>25</v>
@@ -1330,7 +1347,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>29</v>
       </c>
@@ -1351,24 +1368,18 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>34</v>
-      </c>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
-      <c r="G9" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="G9" s="6"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1379,9 +1390,9 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -1392,12 +1403,12 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1409,173 +1420,173 @@
         <v>22</v>
       </c>
       <c r="F12" t="s">
-        <v>8</v>
+        <v>106</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F13" t="s">
-        <v>8</v>
+        <v>106</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E14" t="s">
         <v>23</v>
       </c>
       <c r="F14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F15" t="s">
         <v>11</v>
       </c>
       <c r="G15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>110</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>112</v>
       </c>
       <c r="C18">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D18" t="s">
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="F18" t="s">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="F19" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C20">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="E21" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="F21" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="G21" t="s">
+        <v>61</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -1584,7 +1595,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F22" t="s">
         <v>11</v>
@@ -1592,21 +1603,21 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C23">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F23" t="s">
         <v>8</v>
@@ -1614,31 +1625,31 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D24" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E24" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F24" t="s">
         <v>8</v>
       </c>
       <c r="G24" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C25" s="7">
         <v>1</v>
@@ -1647,7 +1658,7 @@
         <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F25" t="s">
         <v>11</v>
@@ -1655,12 +1666,12 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C26" s="7">
         <v>1</v>
@@ -1669,7 +1680,7 @@
         <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F26" t="s">
         <v>11</v>
@@ -1677,12 +1688,12 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C27" s="7">
         <v>1</v>
@@ -1691,7 +1702,7 @@
         <v>12</v>
       </c>
       <c r="E27" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F27" t="s">
         <v>11</v>
@@ -1699,12 +1710,12 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B28" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C28" s="7">
         <v>1</v>
@@ -1713,7 +1724,7 @@
         <v>12</v>
       </c>
       <c r="E28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="F28" t="s">
         <v>11</v>
@@ -1721,12 +1732,12 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C29" s="7">
         <v>1</v>
@@ -1735,7 +1746,7 @@
         <v>12</v>
       </c>
       <c r="E29" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F29" t="s">
         <v>11</v>
@@ -1743,13 +1754,13 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C30" s="7"/>
       <c r="E30" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F30" t="s">
         <v>11</v>
@@ -1757,21 +1768,21 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B31" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C31" s="7">
         <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E31" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F31" t="s">
         <v>8</v>
@@ -1779,21 +1790,21 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B32" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C32" s="8">
         <v>6</v>
       </c>
       <c r="D32" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E32" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F32" t="s">
         <v>8</v>
@@ -1802,12 +1813,12 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B33" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C33" s="7">
         <v>3</v>
@@ -1816,7 +1827,7 @@
         <v>12</v>
       </c>
       <c r="E33" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="F33" t="s">
         <v>11</v>
@@ -1825,126 +1836,147 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B34" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C34" s="7">
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E34" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F34" t="s">
         <v>8</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D35" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E35" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F35" t="s">
         <v>8</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>104</v>
+      </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>105</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>113</v>
+      </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B39" s="2"/>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B41" s="2"/>
-      <c r="E41" s="3"/>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E43" s="3"/>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="2"/>
+      <c r="E44" s="3"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E45" s="3"/>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="2"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E46" s="3"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="5"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E47" s="3"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="4"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B50" s="1"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B51" s="1"/>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E48" s="3"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E49" s="3"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="5"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E50" s="3"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="1"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="1"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A40:G40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -1953,20 +1985,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="23.5" customWidth="1"/>
-    <col min="5" max="5" width="18.5" customWidth="1"/>
-    <col min="7" max="7" width="59.83203125" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="59.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1989,18 +2023,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -2011,12 +2045,15 @@
       <c r="F4" t="s">
         <v>19</v>
       </c>
+      <c r="G4" t="s">
+        <v>108</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -2025,12 +2062,12 @@
         <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>24</v>
       </c>
@@ -2051,7 +2088,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7" t="s">
         <v>25</v>
@@ -2070,27 +2107,21 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>34</v>
-      </c>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
-      <c r="E8" s="7" t="s">
-        <v>101</v>
-      </c>
+      <c r="E8" s="7"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="6" t="s">
-        <v>106</v>
-      </c>
+      <c r="G8" s="7"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -2100,244 +2131,250 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" t="s">
+        <v>106</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="F11" t="s">
-        <v>8</v>
+        <v>106</v>
+      </c>
+      <c r="G11" t="s">
+        <v>42</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>36</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="F12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>46</v>
-      </c>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>39</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
       <c r="D13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="F13" t="s">
-        <v>40</v>
+        <v>11</v>
+      </c>
+      <c r="G13" t="s">
+        <v>45</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>105</v>
+      </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F14" t="s">
         <v>11</v>
       </c>
-      <c r="G14" t="s">
-        <v>48</v>
-      </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>110</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>112</v>
       </c>
       <c r="C17">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D17" t="s">
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="F17" t="s">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="F18" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F19" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="E20" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F20" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="G20" t="s">
+        <v>61</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>50</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E21" t="s">
-        <v>94</v>
+        <v>51</v>
       </c>
       <c r="F21" t="s">
         <v>8</v>
       </c>
-      <c r="G21" t="s">
-        <v>56</v>
-      </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>72</v>
-      </c>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C22" s="7">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="E22" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F22" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="G22" t="s">
+        <v>53</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C23" s="7">
         <v>1</v>
@@ -2346,7 +2383,7 @@
         <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F23" t="s">
         <v>11</v>
@@ -2354,12 +2391,12 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C24" s="7">
         <v>1</v>
@@ -2368,7 +2405,7 @@
         <v>12</v>
       </c>
       <c r="E24" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="F24" t="s">
         <v>11</v>
@@ -2376,12 +2413,12 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B25" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C25" s="7">
         <v>1</v>
@@ -2390,7 +2427,7 @@
         <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="F25" t="s">
         <v>11</v>
@@ -2398,12 +2435,12 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C26" s="7">
         <v>1</v>
@@ -2412,7 +2449,7 @@
         <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F26" t="s">
         <v>11</v>
@@ -2420,13 +2457,21 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>70</v>
+      </c>
       <c r="B27" t="s">
-        <v>85</v>
-      </c>
-      <c r="C27" s="7"/>
-      <c r="E27" s="3" t="s">
-        <v>101</v>
+        <v>78</v>
+      </c>
+      <c r="C27" s="7">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" t="s">
+        <v>94</v>
       </c>
       <c r="F27" t="s">
         <v>11</v>
@@ -2434,194 +2479,232 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>77</v>
-      </c>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>86</v>
-      </c>
-      <c r="C28" s="7">
-        <v>6</v>
-      </c>
-      <c r="D28" t="s">
-        <v>93</v>
-      </c>
-      <c r="E28" t="s">
-        <v>102</v>
+        <v>79</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="E28" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="F28" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" s="7">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
         <v>87</v>
       </c>
-      <c r="C29" s="8">
-        <v>6</v>
-      </c>
-      <c r="D29" t="s">
-        <v>93</v>
-      </c>
       <c r="E29" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="F29" t="s">
         <v>8</v>
       </c>
-      <c r="G29" s="7"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B30" t="s">
-        <v>112</v>
-      </c>
-      <c r="C30" s="7">
-        <v>3</v>
+        <v>81</v>
+      </c>
+      <c r="C30" s="8">
+        <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="E30" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="F30" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G30" s="7"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B31" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="C31" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E31" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F31" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>92</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="G31" s="7"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>82</v>
+      </c>
       <c r="B32" t="s">
-        <v>90</v>
+        <v>83</v>
+      </c>
+      <c r="C32" s="7">
+        <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E32" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="F32" t="s">
         <v>8</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" t="s">
+        <v>87</v>
+      </c>
+      <c r="E33" t="s">
+        <v>99</v>
+      </c>
+      <c r="F33" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G34" s="6"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G35" s="6"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B36" s="2"/>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" t="s">
+        <v>115</v>
+      </c>
+      <c r="G36" s="6"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B38" s="2"/>
-      <c r="E38" s="3"/>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B39" s="2"/>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E40" s="3"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="2"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="2"/>
       <c r="E42" s="3"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E43" s="3"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="5"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="2"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E44" s="3"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="4"/>
+      <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B47" s="1"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B48" s="1"/>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E46" s="3"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E47" s="3"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="5"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E48" s="3"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="1"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="1"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A38:G38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>